<commit_message>
Add UK countries as dependent territories in inclusion rules
</commit_message>
<xml_diff>
--- a/political-entities.xlsx
+++ b/political-entities.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Axel\Projects\anki-ultimate-geography\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axelb\Projects\anki-ultimate-geography\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2194E189-6E3F-41BF-AF45-9EE97CE7E739}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dependent territories" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
     <sheet name="Transcontinental" sheetId="3" r:id="rId3"/>
     <sheet name="Enclaves and exclaves" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="133">
   <si>
     <t>Territory</t>
   </si>
@@ -414,16 +415,28 @@
   </si>
   <si>
     <t xml:space="preserve">  - pene-enclaves and pene-exclaves</t>
+  </si>
+  <si>
+    <t>England</t>
+  </si>
+  <si>
+    <t>Northern Ireland</t>
+  </si>
+  <si>
+    <t>Scotland</t>
+  </si>
+  <si>
+    <t>Wales</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -475,9 +488,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -500,7 +513,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -537,10 +550,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -567,29 +580,32 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -597,22 +613,12 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="30">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.79998168889431442"/>
@@ -629,14 +635,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -666,6 +665,10 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.79998168889431442"/>
@@ -682,18 +685,15 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.79998168889431442"/>
@@ -710,6 +710,19 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -720,12 +733,6 @@
           <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <font>
@@ -747,22 +754,75 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -846,21 +906,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E39" totalsRowShown="0">
-  <autoFilter ref="A1:E39"/>
-  <sortState ref="A2:E41">
-    <sortCondition ref="D2:D41"/>
-    <sortCondition ref="E2:E41"/>
-    <sortCondition ref="B2:B41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:E43" totalsRowShown="0">
+  <autoFilter ref="A1:E43" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E43">
+    <sortCondition ref="D2:D43"/>
+    <sortCondition ref="E2:E43"/>
+    <sortCondition ref="B2:B43"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="Territory"/>
-    <tableColumn id="2" name="Population" dataDxfId="25" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="Area" dataDxfId="24" dataCellStyle="Comma"/>
-    <tableColumn id="4" name="Location">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Territory"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Population" dataDxfId="26" dataCellStyle="Comma"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Area" dataDxfId="25" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Location">
       <calculatedColumnFormula>IF(OR(Table1[[#This Row],[Population]]&gt;=$I$2,Table1[[#This Row],[Area]]&gt;=$I$3),"YES","NO")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Flag/capital" dataDxfId="23">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Flag/capital" dataDxfId="24">
       <calculatedColumnFormula>IF(OR(AND(Table1[[#This Row],[Population]]&gt;=20000,Table1[[#This Row],[Area]]&gt;=$J$3),Table1[[#This Row],[Population]]&gt;=$K$2,),"YES","NO")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -869,17 +929,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table2" displayName="Table2" ref="A1:D14" totalsRowShown="0">
-  <autoFilter ref="A1:D14"/>
-  <sortState ref="A2:D14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:D14" totalsRowShown="0">
+  <autoFilter ref="A1:D14" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D14">
     <sortCondition ref="D2:D14"/>
     <sortCondition ref="B2:B14"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" name="Territory"/>
-    <tableColumn id="2" name="Population"/>
-    <tableColumn id="3" name="Area"/>
-    <tableColumn id="4" name="Include?" dataDxfId="22">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Territory"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Population"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Area"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Include?" dataDxfId="21">
       <calculatedColumnFormula>IF(Table2[[#This Row],[Population]]&gt;=$H$2,"YES","NO")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -888,20 +948,20 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table3" displayName="Table3" ref="A1:F18" totalsRowShown="0">
-  <autoFilter ref="A1:F18"/>
-  <sortState ref="A2:F17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="A1:F18" totalsRowShown="0">
+  <autoFilter ref="A1:F18" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F17">
     <sortCondition ref="F2:F17" customList="NO,YES"/>
     <sortCondition ref="E2:E17" customList="NA,VERY CLOSE,CLOSE,FAR,VERY FAR"/>
     <sortCondition ref="B2:B17"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="Territory"/>
-    <tableColumn id="2" name="Population" dataDxfId="21" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="Area" dataDxfId="20" dataCellStyle="Comma"/>
-    <tableColumn id="5" name="km" dataDxfId="19"/>
-    <tableColumn id="4" name="Distance"/>
-    <tableColumn id="6" name="Include?">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Territory"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Population" dataDxfId="18" dataCellStyle="Comma"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Area" dataDxfId="17" dataCellStyle="Comma"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="km" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Distance"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Include?">
       <calculatedColumnFormula>IF(AND(Table3[[#This Row],[Population]]&gt;=$J$2,Table3[[#This Row],[Distance]]&lt;&gt;"VERY CLOSE"),"YES","NO")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -910,19 +970,19 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table15" displayName="Table15" ref="A1:E17" totalsRowShown="0">
-  <autoFilter ref="A1:E17"/>
-  <sortState ref="A2:E19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table15" displayName="Table15" ref="A1:E17" totalsRowShown="0">
+  <autoFilter ref="A1:E17" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E19">
     <sortCondition ref="E2:E19"/>
     <sortCondition ref="D2:D19" customList="NA,VERY CLOSE,CLOSE,FAR,VERY FAR"/>
     <sortCondition ref="B2:B19"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="Territory"/>
-    <tableColumn id="3" name="Population" dataDxfId="18" dataCellStyle="Comma"/>
-    <tableColumn id="2" name="Area" dataDxfId="17" dataCellStyle="Comma"/>
-    <tableColumn id="4" name="Distance"/>
-    <tableColumn id="5" name="Include?">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Territory"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Population" dataDxfId="13" dataCellStyle="Comma"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Area" dataDxfId="12" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Distance"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Include?">
       <calculatedColumnFormula>IF(AND(Table15[[#This Row],[Population]]&gt;=$I$2,Table15[[#This Row],[Distance]]&lt;&gt;"VERY CLOSE"),"YES","NO")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1192,10 +1252,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AMK43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1453,13 +1513,13 @@
     </row>
     <row r="11" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="B11" s="34">
-        <v>15100</v>
+        <v>2667</v>
       </c>
       <c r="C11" s="34">
-        <v>91</v>
+        <v>61022</v>
       </c>
       <c r="D11" s="3" t="str">
         <f>IF(OR(Table1[[#This Row],[Population]]&gt;=$I$2,Table1[[#This Row],[Area]]&gt;=$I$3),"YES","NO")</f>
@@ -1472,13 +1532,13 @@
     </row>
     <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="B12" s="34">
-        <v>15664</v>
+        <v>2931</v>
       </c>
       <c r="C12" s="34">
-        <v>142</v>
+        <v>12173</v>
       </c>
       <c r="D12" s="3" t="str">
         <f>IF(OR(Table1[[#This Row],[Population]]&gt;=$I$2,Table1[[#This Row],[Area]]&gt;=$I$3),"YES","NO")</f>
@@ -1491,13 +1551,13 @@
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B13" s="34">
-        <v>15700</v>
+        <v>15100</v>
       </c>
       <c r="C13" s="34">
-        <v>254</v>
+        <v>91</v>
       </c>
       <c r="D13" s="3" t="str">
         <f>IF(OR(Table1[[#This Row],[Population]]&gt;=$I$2,Table1[[#This Row],[Area]]&gt;=$I$3),"YES","NO")</f>
@@ -1510,13 +1570,13 @@
     </row>
     <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B14" s="34">
-        <v>29328</v>
+        <v>15664</v>
       </c>
       <c r="C14" s="34">
-        <v>6.5</v>
+        <v>142</v>
       </c>
       <c r="D14" s="3" t="str">
         <f>IF(OR(Table1[[#This Row],[Population]]&gt;=$I$2,Table1[[#This Row],[Area]]&gt;=$I$3),"YES","NO")</f>
@@ -1529,13 +1589,13 @@
     </row>
     <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B15" s="34">
-        <v>31949</v>
+        <v>15700</v>
       </c>
       <c r="C15" s="34">
-        <v>53.2</v>
+        <v>254</v>
       </c>
       <c r="D15" s="3" t="str">
         <f>IF(OR(Table1[[#This Row],[Population]]&gt;=$I$2,Table1[[#This Row],[Area]]&gt;=$I$3),"YES","NO")</f>
@@ -1548,13 +1608,13 @@
     </row>
     <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B16" s="34">
-        <v>34232</v>
+        <v>29328</v>
       </c>
       <c r="C16" s="34">
-        <v>153</v>
+        <v>6.5</v>
       </c>
       <c r="D16" s="3" t="str">
         <f>IF(OR(Table1[[#This Row],[Population]]&gt;=$I$2,Table1[[#This Row],[Area]]&gt;=$I$3),"YES","NO")</f>
@@ -1567,13 +1627,13 @@
     </row>
     <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B17" s="34">
-        <v>41486</v>
+        <v>31949</v>
       </c>
       <c r="C17" s="34">
-        <v>37</v>
+        <v>53.2</v>
       </c>
       <c r="D17" s="3" t="str">
         <f>IF(OR(Table1[[#This Row],[Population]]&gt;=$I$2,Table1[[#This Row],[Area]]&gt;=$I$3),"YES","NO")</f>
@@ -1586,13 +1646,13 @@
     </row>
     <row r="18" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B18" s="34">
-        <v>51430</v>
+        <v>34232</v>
       </c>
       <c r="C18" s="34">
-        <v>430</v>
+        <v>153</v>
       </c>
       <c r="D18" s="3" t="str">
         <f>IF(OR(Table1[[#This Row],[Population]]&gt;=$I$2,Table1[[#This Row],[Area]]&gt;=$I$3),"YES","NO")</f>
@@ -1605,13 +1665,13 @@
     </row>
     <row r="19" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B19" s="34">
-        <v>53467</v>
+        <v>41486</v>
       </c>
       <c r="C19" s="34">
-        <v>464</v>
+        <v>37</v>
       </c>
       <c r="D19" s="3" t="str">
         <f>IF(OR(Table1[[#This Row],[Population]]&gt;=$I$2,Table1[[#This Row],[Area]]&gt;=$I$3),"YES","NO")</f>
@@ -1624,13 +1684,13 @@
     </row>
     <row r="20" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B20" s="34">
-        <v>54194</v>
+        <v>51430</v>
       </c>
       <c r="C20" s="34">
-        <v>199</v>
+        <v>430</v>
       </c>
       <c r="D20" s="3" t="str">
         <f>IF(OR(Table1[[#This Row],[Population]]&gt;=$I$2,Table1[[#This Row],[Area]]&gt;=$I$3),"YES","NO")</f>
@@ -1643,13 +1703,13 @@
     </row>
     <row r="21" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B21" s="34">
-        <v>57268</v>
+        <v>53467</v>
       </c>
       <c r="C21" s="34">
-        <v>264</v>
+        <v>464</v>
       </c>
       <c r="D21" s="3" t="str">
         <f>IF(OR(Table1[[#This Row],[Population]]&gt;=$I$2,Table1[[#This Row],[Area]]&gt;=$I$3),"YES","NO")</f>
@@ -1662,13 +1722,13 @@
     </row>
     <row r="22" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B22" s="34">
-        <v>63026</v>
+        <v>54194</v>
       </c>
       <c r="C22" s="34">
-        <v>65</v>
+        <v>199</v>
       </c>
       <c r="D22" s="3" t="str">
         <f>IF(OR(Table1[[#This Row],[Population]]&gt;=$I$2,Table1[[#This Row],[Area]]&gt;=$I$3),"YES","NO")</f>
@@ -1681,13 +1741,13 @@
     </row>
     <row r="23" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B23" s="34">
-        <v>70537</v>
+        <v>57268</v>
       </c>
       <c r="C23" s="34">
-        <v>53.2</v>
+        <v>264</v>
       </c>
       <c r="D23" s="3" t="str">
         <f>IF(OR(Table1[[#This Row],[Population]]&gt;=$I$2,Table1[[#This Row],[Area]]&gt;=$I$3),"YES","NO")</f>
@@ -1700,13 +1760,13 @@
     </row>
     <row r="24" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B24" s="34">
-        <v>88195</v>
+        <v>63026</v>
       </c>
       <c r="C24" s="34">
-        <v>572</v>
+        <v>65</v>
       </c>
       <c r="D24" s="3" t="str">
         <f>IF(OR(Table1[[#This Row],[Population]]&gt;=$I$2,Table1[[#This Row],[Area]]&gt;=$I$3),"YES","NO")</f>
@@ -1719,13 +1779,13 @@
     </row>
     <row r="25" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B25" s="34">
-        <v>98069</v>
+        <v>70537</v>
       </c>
       <c r="C25" s="34">
-        <v>118.2</v>
+        <v>53.2</v>
       </c>
       <c r="D25" s="3" t="str">
         <f>IF(OR(Table1[[#This Row],[Population]]&gt;=$I$2,Table1[[#This Row],[Area]]&gt;=$I$3),"YES","NO")</f>
@@ -1738,13 +1798,13 @@
     </row>
     <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B26" s="34">
-        <v>2667</v>
+        <v>88195</v>
       </c>
       <c r="C26" s="34">
-        <v>61022</v>
+        <v>572</v>
       </c>
       <c r="D26" s="3" t="str">
         <f>IF(OR(Table1[[#This Row],[Population]]&gt;=$I$2,Table1[[#This Row],[Area]]&gt;=$I$3),"YES","NO")</f>
@@ -1757,13 +1817,13 @@
     </row>
     <row r="27" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B27" s="34">
-        <v>2931</v>
+        <v>98069</v>
       </c>
       <c r="C27" s="34">
-        <v>12173</v>
+        <v>118.2</v>
       </c>
       <c r="D27" s="3" t="str">
         <f>IF(OR(Table1[[#This Row],[Population]]&gt;=$I$2,Table1[[#This Row],[Area]]&gt;=$I$3),"YES","NO")</f>
@@ -1965,65 +2025,131 @@
       </c>
     </row>
     <row r="38" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="B38" s="34">
-        <v>3411307</v>
-      </c>
-      <c r="C38" s="34">
-        <v>9104</v>
+      <c r="A38" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B38" s="39">
+        <v>1893667</v>
+      </c>
+      <c r="C38" s="39">
+        <v>13562</v>
       </c>
       <c r="D38" s="3" t="str">
         <f>IF(OR(Table1[[#This Row],[Population]]&gt;=$I$2,Table1[[#This Row],[Area]]&gt;=$I$3),"YES","NO")</f>
         <v>YES</v>
       </c>
-      <c r="E38" s="3" t="str">
+      <c r="E38" s="42" t="str">
         <f>IF(OR(AND(Table1[[#This Row],[Population]]&gt;=20000,Table1[[#This Row],[Area]]&gt;=$J$3),Table1[[#This Row],[Population]]&gt;=$K$2,),"YES","NO")</f>
         <v>YES</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="B39" s="34">
-        <v>7374000</v>
-      </c>
-      <c r="C39" s="34">
-        <v>2755</v>
+      <c r="A39" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B39" s="39">
+        <v>3152879</v>
+      </c>
+      <c r="C39" s="39">
+        <v>20735</v>
       </c>
       <c r="D39" s="3" t="str">
         <f>IF(OR(Table1[[#This Row],[Population]]&gt;=$I$2,Table1[[#This Row],[Area]]&gt;=$I$3),"YES","NO")</f>
         <v>YES</v>
       </c>
-      <c r="E39" s="3" t="str">
+      <c r="E39" s="42" t="str">
         <f>IF(OR(AND(Table1[[#This Row],[Population]]&gt;=20000,Table1[[#This Row],[Area]]&gt;=$J$3),Table1[[#This Row],[Population]]&gt;=$K$2,),"YES","NO")</f>
         <v>YES</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="2"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
+      <c r="A40" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B40" s="34">
+        <v>3411307</v>
+      </c>
+      <c r="C40" s="34">
+        <v>9104</v>
+      </c>
+      <c r="D40" s="3" t="str">
+        <f>IF(OR(Table1[[#This Row],[Population]]&gt;=$I$2,Table1[[#This Row],[Area]]&gt;=$I$3),"YES","NO")</f>
+        <v>YES</v>
+      </c>
+      <c r="E40" s="3" t="str">
+        <f>IF(OR(AND(Table1[[#This Row],[Population]]&gt;=20000,Table1[[#This Row],[Area]]&gt;=$J$3),Table1[[#This Row],[Population]]&gt;=$K$2,),"YES","NO")</f>
+        <v>YES</v>
+      </c>
     </row>
     <row r="41" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="2"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
+      <c r="A41" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B41" s="39">
+        <v>5463300</v>
+      </c>
+      <c r="C41" s="39">
+        <v>77933</v>
+      </c>
+      <c r="D41" s="3" t="str">
+        <f>IF(OR(Table1[[#This Row],[Population]]&gt;=$I$2,Table1[[#This Row],[Area]]&gt;=$I$3),"YES","NO")</f>
+        <v>YES</v>
+      </c>
+      <c r="E41" s="42" t="str">
+        <f>IF(OR(AND(Table1[[#This Row],[Population]]&gt;=20000,Table1[[#This Row],[Area]]&gt;=$J$3),Table1[[#This Row],[Population]]&gt;=$K$2,),"YES","NO")</f>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B42" s="34">
+        <v>7374000</v>
+      </c>
+      <c r="C42" s="34">
+        <v>2755</v>
+      </c>
+      <c r="D42" s="3" t="str">
+        <f>IF(OR(Table1[[#This Row],[Population]]&gt;=$I$2,Table1[[#This Row],[Area]]&gt;=$I$3),"YES","NO")</f>
+        <v>YES</v>
+      </c>
+      <c r="E42" s="3" t="str">
+        <f>IF(OR(AND(Table1[[#This Row],[Population]]&gt;=20000,Table1[[#This Row],[Area]]&gt;=$J$3),Table1[[#This Row],[Population]]&gt;=$K$2,),"YES","NO")</f>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B43" s="39">
+        <v>56286961</v>
+      </c>
+      <c r="C43" s="39">
+        <v>130279</v>
+      </c>
+      <c r="D43" s="3" t="str">
+        <f>IF(OR(Table1[[#This Row],[Population]]&gt;=$I$2,Table1[[#This Row],[Area]]&gt;=$I$3),"YES","NO")</f>
+        <v>YES</v>
+      </c>
+      <c r="E43" s="42" t="str">
+        <f>IF(OR(AND(Table1[[#This Row],[Population]]&gt;=20000,Table1[[#This Row],[Area]]&gt;=$J$3),Table1[[#This Row],[Population]]&gt;=$K$2,),"YES","NO")</f>
+        <v>YES</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="J1:K1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A2:A39">
-    <cfRule type="expression" dxfId="8" priority="2">
+  <conditionalFormatting sqref="A2:A43">
+    <cfRule type="expression" dxfId="29" priority="2">
       <formula>$E2="YES"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="28" priority="3">
       <formula>AND($D2="YES",$E2="NO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="27" priority="4">
       <formula>$D2="NO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2036,7 +2162,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
@@ -4328,10 +4454,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A14">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="23" priority="2">
       <formula>$D2="YES"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="22" priority="3">
       <formula>$D2="NO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4344,7 +4470,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMK18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
@@ -7855,10 +7981,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A18">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="20" priority="4">
       <formula>$F2="YES"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="5">
+    <cfRule type="expression" dxfId="19" priority="5">
       <formula>$F2="NO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7871,10 +7997,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8241,10 +8367,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A16">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="15" priority="2">
       <formula>$E2="NO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="14" priority="3">
       <formula>$E2="YES"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>